<commit_message>
Update Prismatica Reference Sheet.xlsx
</commit_message>
<xml_diff>
--- a/Prismatica Reference Sheet.xlsx
+++ b/Prismatica Reference Sheet.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\themy\Documents\GitHub\PrismaGodot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D75728E-722E-488F-A39F-F406A4306508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FAEC81-90F0-47A7-B757-B0B767234C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{FC883E28-E198-4000-AC0F-05D974F02AE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Specialists" sheetId="12" r:id="rId1"/>
-    <sheet name="Skill List" sheetId="16" r:id="rId2"/>
-    <sheet name="Attachments" sheetId="13" r:id="rId3"/>
-    <sheet name="Attachment Values" sheetId="15" r:id="rId4"/>
-    <sheet name="Species Values" sheetId="4" r:id="rId5"/>
-    <sheet name="Species" sheetId="5" r:id="rId6"/>
-    <sheet name="Elements" sheetId="9" r:id="rId7"/>
-    <sheet name="Ranged Weapon" sheetId="10" r:id="rId8"/>
-    <sheet name="Melee Weapon" sheetId="11" r:id="rId9"/>
+    <sheet name="Attachments" sheetId="13" r:id="rId2"/>
+    <sheet name="Attachment Values" sheetId="15" r:id="rId3"/>
+    <sheet name="Species Values" sheetId="4" r:id="rId4"/>
+    <sheet name="Species" sheetId="5" r:id="rId5"/>
+    <sheet name="Elements" sheetId="9" r:id="rId6"/>
+    <sheet name="Ranged Weapon" sheetId="10" r:id="rId7"/>
+    <sheet name="Melee Weapon" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2083" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="513">
   <si>
     <t>HP</t>
   </si>
@@ -12806,42 +12805,6 @@
       </rPr>
       <t>.] (15) {90}</t>
     </r>
-  </si>
-  <si>
-    <t>Species / Skill Category</t>
-  </si>
-  <si>
-    <t>Core</t>
-  </si>
-  <si>
-    <t>Enhancement</t>
-  </si>
-  <si>
-    <t>Mystic</t>
-  </si>
-  <si>
-    <t>Fortification</t>
-  </si>
-  <si>
-    <t>Renewal</t>
-  </si>
-  <si>
-    <t>Evasion</t>
-  </si>
-  <si>
-    <t>Dominion</t>
-  </si>
-  <si>
-    <t>Ascendant</t>
-  </si>
-  <si>
-    <t>Element / Skill Category</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
-    <t>Magic</t>
   </si>
 </sst>
 </file>
@@ -13406,10 +13369,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -13419,21 +13390,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -13445,34 +13414,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="14" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="15" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -13484,8 +13432,23 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -14655,36 +14618,36 @@
       <c r="B28" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="C28" s="83" t="s">
+      <c r="C28" s="91" t="s">
         <v>264</v>
       </c>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="85"/>
+      <c r="D28" s="92"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="93"/>
       <c r="I28" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="J28" s="81" t="s">
+      <c r="J28" s="90" t="s">
         <v>265</v>
       </c>
-      <c r="K28" s="81"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="81"/>
-      <c r="N28" s="81"/>
-      <c r="O28" s="81"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
       <c r="P28" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="Q28" s="81" t="s">
+      <c r="Q28" s="90" t="s">
         <v>266</v>
       </c>
-      <c r="R28" s="81"/>
-      <c r="S28" s="81"/>
-      <c r="T28" s="81"/>
-      <c r="U28" s="81"/>
-      <c r="V28" s="81"/>
+      <c r="R28" s="90"/>
+      <c r="S28" s="90"/>
+      <c r="T28" s="90"/>
+      <c r="U28" s="90"/>
+      <c r="V28" s="90"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
@@ -14693,36 +14656,36 @@
       <c r="B29" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C29" s="89" t="s">
+      <c r="C29" s="94" t="s">
         <v>507</v>
       </c>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="91"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="96"/>
       <c r="I29" s="58" t="s">
         <v>489</v>
       </c>
-      <c r="J29" s="92" t="s">
+      <c r="J29" s="86" t="s">
         <v>375</v>
       </c>
-      <c r="K29" s="92"/>
-      <c r="L29" s="92"/>
-      <c r="M29" s="92"/>
-      <c r="N29" s="92"/>
-      <c r="O29" s="92"/>
+      <c r="K29" s="86"/>
+      <c r="L29" s="86"/>
+      <c r="M29" s="86"/>
+      <c r="N29" s="86"/>
+      <c r="O29" s="86"/>
       <c r="P29" s="58" t="s">
         <v>490</v>
       </c>
-      <c r="Q29" s="92" t="s">
+      <c r="Q29" s="86" t="s">
         <v>392</v>
       </c>
-      <c r="R29" s="92"/>
-      <c r="S29" s="92"/>
-      <c r="T29" s="92"/>
-      <c r="U29" s="92"/>
-      <c r="V29" s="92"/>
+      <c r="R29" s="86"/>
+      <c r="S29" s="86"/>
+      <c r="T29" s="86"/>
+      <c r="U29" s="86"/>
+      <c r="V29" s="86"/>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
@@ -14731,14 +14694,14 @@
       <c r="B30" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="83" t="s">
         <v>497</v>
       </c>
-      <c r="D30" s="87"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="88"/>
+      <c r="D30" s="84"/>
+      <c r="E30" s="84"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="85"/>
       <c r="I30" s="58" t="s">
         <v>489</v>
       </c>
@@ -14769,14 +14732,14 @@
       <c r="B31" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C31" s="86" t="s">
+      <c r="C31" s="83" t="s">
         <v>369</v>
       </c>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="88"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="85"/>
       <c r="I31" s="58" t="s">
         <v>489</v>
       </c>
@@ -14807,14 +14770,14 @@
       <c r="B32" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C32" s="86" t="s">
+      <c r="C32" s="83" t="s">
         <v>370</v>
       </c>
-      <c r="D32" s="87"/>
-      <c r="E32" s="87"/>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
-      <c r="H32" s="88"/>
+      <c r="D32" s="84"/>
+      <c r="E32" s="84"/>
+      <c r="F32" s="84"/>
+      <c r="G32" s="84"/>
+      <c r="H32" s="85"/>
       <c r="I32" s="58" t="s">
         <v>489</v>
       </c>
@@ -14845,14 +14808,14 @@
       <c r="B33" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C33" s="86" t="s">
+      <c r="C33" s="83" t="s">
         <v>504</v>
       </c>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="88"/>
+      <c r="D33" s="84"/>
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="84"/>
+      <c r="H33" s="85"/>
       <c r="I33" s="58" t="s">
         <v>489</v>
       </c>
@@ -14883,14 +14846,14 @@
       <c r="B34" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C34" s="86" t="s">
+      <c r="C34" s="83" t="s">
         <v>505</v>
       </c>
-      <c r="D34" s="87"/>
-      <c r="E34" s="87"/>
-      <c r="F34" s="87"/>
-      <c r="G34" s="87"/>
-      <c r="H34" s="88"/>
+      <c r="D34" s="84"/>
+      <c r="E34" s="84"/>
+      <c r="F34" s="84"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="85"/>
       <c r="I34" s="58" t="s">
         <v>489</v>
       </c>
@@ -14921,14 +14884,14 @@
       <c r="B35" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C35" s="86" t="s">
+      <c r="C35" s="83" t="s">
         <v>506</v>
       </c>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="88"/>
+      <c r="D35" s="84"/>
+      <c r="E35" s="84"/>
+      <c r="F35" s="84"/>
+      <c r="G35" s="84"/>
+      <c r="H35" s="85"/>
       <c r="I35" s="58" t="s">
         <v>489</v>
       </c>
@@ -14959,14 +14922,14 @@
       <c r="B36" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C36" s="86" t="s">
+      <c r="C36" s="83" t="s">
         <v>389</v>
       </c>
-      <c r="D36" s="87"/>
-      <c r="E36" s="87"/>
-      <c r="F36" s="87"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="88"/>
+      <c r="D36" s="84"/>
+      <c r="E36" s="84"/>
+      <c r="F36" s="84"/>
+      <c r="G36" s="84"/>
+      <c r="H36" s="85"/>
       <c r="I36" s="58" t="s">
         <v>489</v>
       </c>
@@ -14997,14 +14960,14 @@
       <c r="B37" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C37" s="86" t="s">
+      <c r="C37" s="83" t="s">
         <v>496</v>
       </c>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="88"/>
+      <c r="D37" s="84"/>
+      <c r="E37" s="84"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="85"/>
       <c r="I37" s="58" t="s">
         <v>489</v>
       </c>
@@ -15035,14 +14998,14 @@
       <c r="B38" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C38" s="86" t="s">
+      <c r="C38" s="83" t="s">
         <v>510</v>
       </c>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
-      <c r="H38" s="88"/>
+      <c r="D38" s="84"/>
+      <c r="E38" s="84"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="85"/>
       <c r="I38" s="58" t="s">
         <v>489</v>
       </c>
@@ -15073,14 +15036,14 @@
       <c r="B39" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C39" s="86" t="s">
+      <c r="C39" s="83" t="s">
         <v>373</v>
       </c>
-      <c r="D39" s="87"/>
-      <c r="E39" s="87"/>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87"/>
-      <c r="H39" s="88"/>
+      <c r="D39" s="84"/>
+      <c r="E39" s="84"/>
+      <c r="F39" s="84"/>
+      <c r="G39" s="84"/>
+      <c r="H39" s="85"/>
       <c r="I39" s="58" t="s">
         <v>489</v>
       </c>
@@ -15111,14 +15074,14 @@
       <c r="B40" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C40" s="86" t="s">
+      <c r="C40" s="83" t="s">
         <v>503</v>
       </c>
-      <c r="D40" s="87"/>
-      <c r="E40" s="87"/>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
-      <c r="H40" s="88"/>
+      <c r="D40" s="84"/>
+      <c r="E40" s="84"/>
+      <c r="F40" s="84"/>
+      <c r="G40" s="84"/>
+      <c r="H40" s="85"/>
       <c r="I40" s="58" t="s">
         <v>489</v>
       </c>
@@ -15149,14 +15112,14 @@
       <c r="B41" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C41" s="86" t="s">
+      <c r="C41" s="83" t="s">
         <v>368</v>
       </c>
-      <c r="D41" s="87"/>
-      <c r="E41" s="87"/>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
-      <c r="H41" s="88"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="85"/>
       <c r="I41" s="58" t="s">
         <v>489</v>
       </c>
@@ -15187,14 +15150,14 @@
       <c r="B42" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C42" s="86" t="s">
+      <c r="C42" s="83" t="s">
         <v>508</v>
       </c>
-      <c r="D42" s="87"/>
-      <c r="E42" s="87"/>
-      <c r="F42" s="87"/>
-      <c r="G42" s="87"/>
-      <c r="H42" s="88"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="84"/>
+      <c r="F42" s="84"/>
+      <c r="G42" s="84"/>
+      <c r="H42" s="85"/>
       <c r="I42" s="58" t="s">
         <v>489</v>
       </c>
@@ -15225,14 +15188,14 @@
       <c r="B43" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C43" s="86" t="s">
+      <c r="C43" s="83" t="s">
         <v>509</v>
       </c>
-      <c r="D43" s="87"/>
-      <c r="E43" s="87"/>
-      <c r="F43" s="87"/>
-      <c r="G43" s="87"/>
-      <c r="H43" s="88"/>
+      <c r="D43" s="84"/>
+      <c r="E43" s="84"/>
+      <c r="F43" s="84"/>
+      <c r="G43" s="84"/>
+      <c r="H43" s="85"/>
       <c r="I43" s="58" t="s">
         <v>489</v>
       </c>
@@ -15263,14 +15226,14 @@
       <c r="B44" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="83" t="s">
         <v>371</v>
       </c>
-      <c r="D44" s="87"/>
-      <c r="E44" s="87"/>
-      <c r="F44" s="87"/>
-      <c r="G44" s="87"/>
-      <c r="H44" s="88"/>
+      <c r="D44" s="84"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="84"/>
+      <c r="G44" s="84"/>
+      <c r="H44" s="85"/>
       <c r="I44" s="58" t="s">
         <v>489</v>
       </c>
@@ -15301,14 +15264,14 @@
       <c r="B45" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C45" s="86" t="s">
+      <c r="C45" s="83" t="s">
         <v>502</v>
       </c>
-      <c r="D45" s="87"/>
-      <c r="E45" s="87"/>
-      <c r="F45" s="87"/>
-      <c r="G45" s="87"/>
-      <c r="H45" s="88"/>
+      <c r="D45" s="84"/>
+      <c r="E45" s="84"/>
+      <c r="F45" s="84"/>
+      <c r="G45" s="84"/>
+      <c r="H45" s="85"/>
       <c r="I45" s="58" t="s">
         <v>489</v>
       </c>
@@ -15339,14 +15302,14 @@
       <c r="B46" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C46" s="86" t="s">
+      <c r="C46" s="83" t="s">
         <v>501</v>
       </c>
-      <c r="D46" s="87"/>
-      <c r="E46" s="87"/>
-      <c r="F46" s="87"/>
-      <c r="G46" s="87"/>
-      <c r="H46" s="88"/>
+      <c r="D46" s="84"/>
+      <c r="E46" s="84"/>
+      <c r="F46" s="84"/>
+      <c r="G46" s="84"/>
+      <c r="H46" s="85"/>
       <c r="I46" s="58" t="s">
         <v>489</v>
       </c>
@@ -15377,14 +15340,14 @@
       <c r="B47" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C47" s="86" t="s">
+      <c r="C47" s="83" t="s">
         <v>372</v>
       </c>
-      <c r="D47" s="87"/>
-      <c r="E47" s="87"/>
-      <c r="F47" s="87"/>
-      <c r="G47" s="87"/>
-      <c r="H47" s="88"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
+      <c r="F47" s="84"/>
+      <c r="G47" s="84"/>
+      <c r="H47" s="85"/>
       <c r="I47" s="58" t="s">
         <v>489</v>
       </c>
@@ -15415,14 +15378,14 @@
       <c r="B48" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C48" s="86" t="s">
+      <c r="C48" s="83" t="s">
         <v>500</v>
       </c>
-      <c r="D48" s="87"/>
-      <c r="E48" s="87"/>
-      <c r="F48" s="87"/>
-      <c r="G48" s="87"/>
-      <c r="H48" s="88"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="84"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="85"/>
       <c r="I48" s="58" t="s">
         <v>489</v>
       </c>
@@ -15453,14 +15416,14 @@
       <c r="B49" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C49" s="86" t="s">
+      <c r="C49" s="83" t="s">
         <v>366</v>
       </c>
-      <c r="D49" s="87"/>
-      <c r="E49" s="87"/>
-      <c r="F49" s="87"/>
-      <c r="G49" s="87"/>
-      <c r="H49" s="88"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="84"/>
+      <c r="G49" s="84"/>
+      <c r="H49" s="85"/>
       <c r="I49" s="58" t="s">
         <v>489</v>
       </c>
@@ -15491,14 +15454,14 @@
       <c r="B50" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C50" s="86" t="s">
+      <c r="C50" s="83" t="s">
         <v>367</v>
       </c>
-      <c r="D50" s="87"/>
-      <c r="E50" s="87"/>
-      <c r="F50" s="87"/>
-      <c r="G50" s="87"/>
-      <c r="H50" s="88"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="84"/>
+      <c r="F50" s="84"/>
+      <c r="G50" s="84"/>
+      <c r="H50" s="85"/>
       <c r="I50" s="58" t="s">
         <v>489</v>
       </c>
@@ -15529,14 +15492,14 @@
       <c r="B51" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C51" s="86" t="s">
+      <c r="C51" s="83" t="s">
         <v>374</v>
       </c>
-      <c r="D51" s="87"/>
-      <c r="E51" s="87"/>
-      <c r="F51" s="87"/>
-      <c r="G51" s="87"/>
-      <c r="H51" s="88"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="84"/>
+      <c r="F51" s="84"/>
+      <c r="G51" s="84"/>
+      <c r="H51" s="85"/>
       <c r="I51" s="58" t="s">
         <v>489</v>
       </c>
@@ -15567,14 +15530,14 @@
       <c r="B52" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C52" s="86" t="s">
+      <c r="C52" s="83" t="s">
         <v>499</v>
       </c>
-      <c r="D52" s="87"/>
-      <c r="E52" s="87"/>
-      <c r="F52" s="87"/>
-      <c r="G52" s="87"/>
-      <c r="H52" s="88"/>
+      <c r="D52" s="84"/>
+      <c r="E52" s="84"/>
+      <c r="F52" s="84"/>
+      <c r="G52" s="84"/>
+      <c r="H52" s="85"/>
       <c r="I52" s="58" t="s">
         <v>489</v>
       </c>
@@ -15605,36 +15568,36 @@
       <c r="B53" s="58" t="s">
         <v>488</v>
       </c>
-      <c r="C53" s="94" t="s">
+      <c r="C53" s="87" t="s">
         <v>498</v>
       </c>
-      <c r="D53" s="95"/>
-      <c r="E53" s="95"/>
-      <c r="F53" s="95"/>
-      <c r="G53" s="95"/>
-      <c r="H53" s="96"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="88"/>
+      <c r="F53" s="88"/>
+      <c r="G53" s="88"/>
+      <c r="H53" s="89"/>
       <c r="I53" s="58" t="s">
         <v>489</v>
       </c>
-      <c r="J53" s="93" t="s">
+      <c r="J53" s="81" t="s">
         <v>377</v>
       </c>
-      <c r="K53" s="93"/>
-      <c r="L53" s="93"/>
-      <c r="M53" s="93"/>
-      <c r="N53" s="93"/>
-      <c r="O53" s="93"/>
+      <c r="K53" s="81"/>
+      <c r="L53" s="81"/>
+      <c r="M53" s="81"/>
+      <c r="N53" s="81"/>
+      <c r="O53" s="81"/>
       <c r="P53" s="58" t="s">
         <v>490</v>
       </c>
-      <c r="Q53" s="93" t="s">
+      <c r="Q53" s="81" t="s">
         <v>399</v>
       </c>
-      <c r="R53" s="93"/>
-      <c r="S53" s="93"/>
-      <c r="T53" s="93"/>
-      <c r="U53" s="93"/>
-      <c r="V53" s="93"/>
+      <c r="R53" s="81"/>
+      <c r="S53" s="81"/>
+      <c r="T53" s="81"/>
+      <c r="U53" s="81"/>
+      <c r="V53" s="81"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="80"/>
@@ -15664,36 +15627,36 @@
       <c r="B55" s="23" t="s">
         <v>491</v>
       </c>
-      <c r="C55" s="81" t="s">
+      <c r="C55" s="90" t="s">
         <v>267</v>
       </c>
-      <c r="D55" s="81"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="81"/>
-      <c r="G55" s="81"/>
-      <c r="H55" s="81"/>
+      <c r="D55" s="90"/>
+      <c r="E55" s="90"/>
+      <c r="F55" s="90"/>
+      <c r="G55" s="90"/>
+      <c r="H55" s="90"/>
       <c r="I55" s="23" t="s">
         <v>491</v>
       </c>
-      <c r="J55" s="81" t="s">
+      <c r="J55" s="90" t="s">
         <v>268</v>
       </c>
-      <c r="K55" s="81"/>
-      <c r="L55" s="81"/>
-      <c r="M55" s="81"/>
-      <c r="N55" s="81"/>
-      <c r="O55" s="81"/>
+      <c r="K55" s="90"/>
+      <c r="L55" s="90"/>
+      <c r="M55" s="90"/>
+      <c r="N55" s="90"/>
+      <c r="O55" s="90"/>
       <c r="P55" s="23" t="s">
         <v>491</v>
       </c>
-      <c r="Q55" s="81" t="s">
+      <c r="Q55" s="90" t="s">
         <v>269</v>
       </c>
-      <c r="R55" s="81"/>
-      <c r="S55" s="81"/>
-      <c r="T55" s="81"/>
-      <c r="U55" s="81"/>
-      <c r="V55" s="81"/>
+      <c r="R55" s="90"/>
+      <c r="S55" s="90"/>
+      <c r="T55" s="90"/>
+      <c r="U55" s="90"/>
+      <c r="V55" s="90"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="s">
@@ -15702,36 +15665,36 @@
       <c r="B56" s="31" t="s">
         <v>495</v>
       </c>
-      <c r="C56" s="92" t="s">
+      <c r="C56" s="86" t="s">
         <v>430</v>
       </c>
-      <c r="D56" s="92"/>
-      <c r="E56" s="92"/>
-      <c r="F56" s="92"/>
-      <c r="G56" s="92"/>
-      <c r="H56" s="92"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="86"/>
+      <c r="G56" s="86"/>
+      <c r="H56" s="86"/>
       <c r="I56" s="31" t="s">
         <v>348</v>
       </c>
-      <c r="J56" s="92" t="s">
+      <c r="J56" s="86" t="s">
         <v>439</v>
       </c>
-      <c r="K56" s="92"/>
-      <c r="L56" s="92"/>
-      <c r="M56" s="92"/>
-      <c r="N56" s="92"/>
-      <c r="O56" s="92"/>
+      <c r="K56" s="86"/>
+      <c r="L56" s="86"/>
+      <c r="M56" s="86"/>
+      <c r="N56" s="86"/>
+      <c r="O56" s="86"/>
       <c r="P56" s="31" t="s">
         <v>492</v>
       </c>
-      <c r="Q56" s="92" t="s">
+      <c r="Q56" s="86" t="s">
         <v>511</v>
       </c>
-      <c r="R56" s="92"/>
-      <c r="S56" s="92"/>
-      <c r="T56" s="92"/>
-      <c r="U56" s="92"/>
-      <c r="V56" s="92"/>
+      <c r="R56" s="86"/>
+      <c r="S56" s="86"/>
+      <c r="T56" s="86"/>
+      <c r="U56" s="86"/>
+      <c r="V56" s="86"/>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
@@ -16614,51 +16577,159 @@
       <c r="B80" s="28" t="s">
         <v>495</v>
       </c>
-      <c r="C80" s="93" t="s">
+      <c r="C80" s="81" t="s">
         <v>468</v>
       </c>
-      <c r="D80" s="93"/>
-      <c r="E80" s="93"/>
-      <c r="F80" s="93"/>
-      <c r="G80" s="93"/>
-      <c r="H80" s="93"/>
+      <c r="D80" s="81"/>
+      <c r="E80" s="81"/>
+      <c r="F80" s="81"/>
+      <c r="G80" s="81"/>
+      <c r="H80" s="81"/>
       <c r="I80" s="28" t="s">
         <v>348</v>
       </c>
-      <c r="J80" s="93" t="s">
+      <c r="J80" s="81" t="s">
         <v>454</v>
       </c>
-      <c r="K80" s="93"/>
-      <c r="L80" s="93"/>
-      <c r="M80" s="93"/>
-      <c r="N80" s="93"/>
-      <c r="O80" s="93"/>
+      <c r="K80" s="81"/>
+      <c r="L80" s="81"/>
+      <c r="M80" s="81"/>
+      <c r="N80" s="81"/>
+      <c r="O80" s="81"/>
       <c r="P80" s="28" t="s">
         <v>492</v>
       </c>
-      <c r="Q80" s="93" t="s">
+      <c r="Q80" s="81" t="s">
         <v>486</v>
       </c>
-      <c r="R80" s="93"/>
-      <c r="S80" s="93"/>
-      <c r="T80" s="93"/>
-      <c r="U80" s="93"/>
-      <c r="V80" s="93"/>
+      <c r="R80" s="81"/>
+      <c r="S80" s="81"/>
+      <c r="T80" s="81"/>
+      <c r="U80" s="81"/>
+      <c r="V80" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="156">
-    <mergeCell ref="J53:O53"/>
-    <mergeCell ref="Q46:V46"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="J49:O49"/>
-    <mergeCell ref="J51:O51"/>
-    <mergeCell ref="Q52:V52"/>
-    <mergeCell ref="Q53:V53"/>
-    <mergeCell ref="C52:H52"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="Q50:V50"/>
-    <mergeCell ref="Q51:V51"/>
-    <mergeCell ref="J50:O50"/>
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="J48:O48"/>
+    <mergeCell ref="J42:O42"/>
+    <mergeCell ref="Q28:V28"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="J43:O43"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="J47:O47"/>
+    <mergeCell ref="Q38:V38"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="J29:O29"/>
+    <mergeCell ref="J39:O39"/>
+    <mergeCell ref="Q30:V30"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="J35:O35"/>
+    <mergeCell ref="J30:O30"/>
+    <mergeCell ref="Q40:V40"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="J31:O31"/>
+    <mergeCell ref="Q42:V42"/>
+    <mergeCell ref="C38:H38"/>
+    <mergeCell ref="J37:O37"/>
+    <mergeCell ref="C71:H71"/>
+    <mergeCell ref="J60:O60"/>
+    <mergeCell ref="Q75:V75"/>
+    <mergeCell ref="C76:H76"/>
+    <mergeCell ref="J62:O62"/>
+    <mergeCell ref="C59:H59"/>
+    <mergeCell ref="J69:O69"/>
+    <mergeCell ref="C55:H55"/>
+    <mergeCell ref="J55:O55"/>
+    <mergeCell ref="Q55:V55"/>
+    <mergeCell ref="Q61:V61"/>
+    <mergeCell ref="Q56:V56"/>
+    <mergeCell ref="Q58:V58"/>
+    <mergeCell ref="C56:H56"/>
+    <mergeCell ref="C58:H58"/>
+    <mergeCell ref="C66:H66"/>
+    <mergeCell ref="J58:O58"/>
+    <mergeCell ref="C72:H72"/>
+    <mergeCell ref="C57:H57"/>
+    <mergeCell ref="J67:O67"/>
+    <mergeCell ref="Q60:V60"/>
+    <mergeCell ref="C62:H62"/>
+    <mergeCell ref="J72:O72"/>
+    <mergeCell ref="C61:H61"/>
+    <mergeCell ref="Q79:V79"/>
+    <mergeCell ref="C79:H79"/>
+    <mergeCell ref="J56:O56"/>
+    <mergeCell ref="Q65:V65"/>
+    <mergeCell ref="C63:H63"/>
+    <mergeCell ref="J66:O66"/>
+    <mergeCell ref="Q74:V74"/>
+    <mergeCell ref="C64:H64"/>
+    <mergeCell ref="J59:O59"/>
+    <mergeCell ref="Q57:V57"/>
+    <mergeCell ref="C77:H77"/>
+    <mergeCell ref="J65:O65"/>
+    <mergeCell ref="Q70:V70"/>
+    <mergeCell ref="C60:H60"/>
+    <mergeCell ref="J68:O68"/>
+    <mergeCell ref="Q69:V69"/>
+    <mergeCell ref="C73:H73"/>
+    <mergeCell ref="J57:O57"/>
+    <mergeCell ref="Q64:V64"/>
+    <mergeCell ref="J61:O61"/>
+    <mergeCell ref="Q76:V76"/>
+    <mergeCell ref="C74:H74"/>
+    <mergeCell ref="J71:O71"/>
+    <mergeCell ref="Q72:V72"/>
+    <mergeCell ref="J74:O74"/>
+    <mergeCell ref="Q66:V66"/>
+    <mergeCell ref="Q62:V62"/>
+    <mergeCell ref="Q59:V59"/>
+    <mergeCell ref="C70:H70"/>
+    <mergeCell ref="Q63:V63"/>
+    <mergeCell ref="C80:H80"/>
+    <mergeCell ref="J63:O63"/>
+    <mergeCell ref="Q71:V71"/>
+    <mergeCell ref="C75:H75"/>
+    <mergeCell ref="J73:O73"/>
+    <mergeCell ref="C69:H69"/>
+    <mergeCell ref="J76:O76"/>
+    <mergeCell ref="Q73:V73"/>
+    <mergeCell ref="C65:H65"/>
+    <mergeCell ref="J64:O64"/>
+    <mergeCell ref="C68:H68"/>
+    <mergeCell ref="J78:O78"/>
+    <mergeCell ref="Q67:V67"/>
+    <mergeCell ref="J75:O75"/>
+    <mergeCell ref="Q68:V68"/>
+    <mergeCell ref="J77:O77"/>
+    <mergeCell ref="Q80:V80"/>
+    <mergeCell ref="C78:H78"/>
+    <mergeCell ref="J70:O70"/>
+    <mergeCell ref="Q78:V78"/>
+    <mergeCell ref="C67:H67"/>
+    <mergeCell ref="Q77:V77"/>
+    <mergeCell ref="J80:O80"/>
+    <mergeCell ref="J79:O79"/>
+    <mergeCell ref="Q29:V29"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="Q36:V36"/>
+    <mergeCell ref="C53:H53"/>
+    <mergeCell ref="J33:O33"/>
+    <mergeCell ref="Q34:V34"/>
+    <mergeCell ref="Q31:V31"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="Q33:V33"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="Q39:V39"/>
+    <mergeCell ref="C49:H49"/>
+    <mergeCell ref="J38:O38"/>
+    <mergeCell ref="Q47:V47"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C31:H31"/>
     <mergeCell ref="Q32:V32"/>
     <mergeCell ref="C34:H34"/>
     <mergeCell ref="J45:O45"/>
@@ -16683,126 +16754,18 @@
     <mergeCell ref="C35:H35"/>
     <mergeCell ref="Q44:V44"/>
     <mergeCell ref="J40:O40"/>
-    <mergeCell ref="J70:O70"/>
-    <mergeCell ref="Q78:V78"/>
-    <mergeCell ref="C67:H67"/>
-    <mergeCell ref="Q77:V77"/>
-    <mergeCell ref="J80:O80"/>
-    <mergeCell ref="J79:O79"/>
-    <mergeCell ref="Q29:V29"/>
-    <mergeCell ref="C33:H33"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="Q36:V36"/>
-    <mergeCell ref="C53:H53"/>
-    <mergeCell ref="J33:O33"/>
-    <mergeCell ref="Q34:V34"/>
-    <mergeCell ref="Q31:V31"/>
-    <mergeCell ref="C39:H39"/>
-    <mergeCell ref="J44:O44"/>
-    <mergeCell ref="Q33:V33"/>
-    <mergeCell ref="C50:H50"/>
-    <mergeCell ref="Q39:V39"/>
-    <mergeCell ref="C49:H49"/>
-    <mergeCell ref="J38:O38"/>
-    <mergeCell ref="Q47:V47"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="J74:O74"/>
-    <mergeCell ref="Q66:V66"/>
-    <mergeCell ref="Q62:V62"/>
-    <mergeCell ref="Q59:V59"/>
-    <mergeCell ref="C70:H70"/>
-    <mergeCell ref="Q63:V63"/>
-    <mergeCell ref="C80:H80"/>
-    <mergeCell ref="J63:O63"/>
-    <mergeCell ref="Q71:V71"/>
-    <mergeCell ref="C75:H75"/>
-    <mergeCell ref="J73:O73"/>
-    <mergeCell ref="C69:H69"/>
-    <mergeCell ref="J76:O76"/>
-    <mergeCell ref="Q73:V73"/>
-    <mergeCell ref="C65:H65"/>
-    <mergeCell ref="J64:O64"/>
-    <mergeCell ref="C68:H68"/>
-    <mergeCell ref="J78:O78"/>
-    <mergeCell ref="Q67:V67"/>
-    <mergeCell ref="J75:O75"/>
-    <mergeCell ref="Q68:V68"/>
-    <mergeCell ref="J77:O77"/>
-    <mergeCell ref="Q80:V80"/>
-    <mergeCell ref="C78:H78"/>
-    <mergeCell ref="Q79:V79"/>
-    <mergeCell ref="C79:H79"/>
-    <mergeCell ref="J56:O56"/>
-    <mergeCell ref="Q65:V65"/>
-    <mergeCell ref="C63:H63"/>
-    <mergeCell ref="J66:O66"/>
-    <mergeCell ref="Q74:V74"/>
-    <mergeCell ref="C64:H64"/>
-    <mergeCell ref="J59:O59"/>
-    <mergeCell ref="Q57:V57"/>
-    <mergeCell ref="C77:H77"/>
-    <mergeCell ref="J65:O65"/>
-    <mergeCell ref="Q70:V70"/>
-    <mergeCell ref="C60:H60"/>
-    <mergeCell ref="J68:O68"/>
-    <mergeCell ref="Q69:V69"/>
-    <mergeCell ref="C73:H73"/>
-    <mergeCell ref="J57:O57"/>
-    <mergeCell ref="Q64:V64"/>
-    <mergeCell ref="J61:O61"/>
-    <mergeCell ref="Q76:V76"/>
-    <mergeCell ref="C74:H74"/>
-    <mergeCell ref="J71:O71"/>
-    <mergeCell ref="Q72:V72"/>
-    <mergeCell ref="C71:H71"/>
-    <mergeCell ref="J60:O60"/>
-    <mergeCell ref="Q75:V75"/>
-    <mergeCell ref="C76:H76"/>
-    <mergeCell ref="J62:O62"/>
-    <mergeCell ref="C59:H59"/>
-    <mergeCell ref="J69:O69"/>
-    <mergeCell ref="C55:H55"/>
-    <mergeCell ref="J55:O55"/>
-    <mergeCell ref="Q55:V55"/>
-    <mergeCell ref="Q61:V61"/>
-    <mergeCell ref="Q56:V56"/>
-    <mergeCell ref="Q58:V58"/>
-    <mergeCell ref="C56:H56"/>
-    <mergeCell ref="C58:H58"/>
-    <mergeCell ref="C66:H66"/>
-    <mergeCell ref="J58:O58"/>
-    <mergeCell ref="C72:H72"/>
-    <mergeCell ref="C57:H57"/>
-    <mergeCell ref="J67:O67"/>
-    <mergeCell ref="Q60:V60"/>
-    <mergeCell ref="C62:H62"/>
-    <mergeCell ref="J72:O72"/>
-    <mergeCell ref="C61:H61"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="J48:O48"/>
-    <mergeCell ref="J42:O42"/>
-    <mergeCell ref="Q28:V28"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="J43:O43"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="J47:O47"/>
-    <mergeCell ref="Q38:V38"/>
-    <mergeCell ref="C43:H43"/>
-    <mergeCell ref="J29:O29"/>
-    <mergeCell ref="J39:O39"/>
-    <mergeCell ref="Q30:V30"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="J35:O35"/>
-    <mergeCell ref="J30:O30"/>
-    <mergeCell ref="Q40:V40"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="J31:O31"/>
-    <mergeCell ref="Q42:V42"/>
-    <mergeCell ref="C38:H38"/>
-    <mergeCell ref="J37:O37"/>
+    <mergeCell ref="J53:O53"/>
+    <mergeCell ref="Q46:V46"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="J49:O49"/>
+    <mergeCell ref="J51:O51"/>
+    <mergeCell ref="Q52:V52"/>
+    <mergeCell ref="Q53:V53"/>
+    <mergeCell ref="C52:H52"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="Q50:V50"/>
+    <mergeCell ref="Q51:V51"/>
+    <mergeCell ref="J50:O50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16810,163 +16773,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCEDB81C-BC5D-42C0-BE0C-3BA57B4D4522}">
-  <dimension ref="A1:K19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="11" width="30.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>513</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>522</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F11" t="s">
-        <v>95</v>
-      </c>
-      <c r="G11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" t="s">
-        <v>98</v>
-      </c>
-      <c r="J11" t="s">
-        <v>523</v>
-      </c>
-      <c r="K11" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>521</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0410F4C1-7835-0A40-ABB1-E2B2F6A7F2C7}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17613,7 +17423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66057716-A026-4C72-ABAA-378493C99A60}">
   <dimension ref="A1:E38"/>
   <sheetViews>
@@ -17755,19 +17565,19 @@
       <c r="A13" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="101" t="s">
         <v>280</v>
       </c>
-      <c r="C13" s="99"/>
+      <c r="C13" s="101"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="102" t="s">
         <v>281</v>
       </c>
-      <c r="C14" s="101"/>
+      <c r="C14" s="103"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="74" t="s">
@@ -17980,21 +17790,19 @@
       <c r="A38" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="102" t="s">
+      <c r="B38" s="99" t="s">
         <v>290</v>
       </c>
-      <c r="C38" s="103"/>
+      <c r="C38" s="100"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
@@ -18007,19 +17815,21 @@
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245A369E-F8D4-413B-A54E-BBAD732E8CBE}">
   <dimension ref="A1:N35"/>
   <sheetViews>
@@ -19002,7 +18812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A232F90D-A2DC-47ED-83E3-098C14BC64FC}">
   <dimension ref="A1:M6"/>
   <sheetViews>
@@ -19265,7 +19075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71E2540-F95E-4A8F-9A85-F586C8A75A79}">
   <dimension ref="A1:M82"/>
   <sheetViews>
@@ -20483,7 +20293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C93BE42-F723-4518-B894-C497BFBFCD2A}">
   <dimension ref="A1:W277"/>
   <sheetViews>
@@ -20500,7 +20310,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="113" t="s">
         <v>156</v>
       </c>
       <c r="B1" s="62" t="s">
@@ -20553,7 +20363,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="105"/>
+      <c r="A2" s="114"/>
       <c r="B2" s="63">
         <v>100</v>
       </c>
@@ -22552,7 +22362,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="106" t="s">
+      <c r="A39" s="111" t="s">
         <v>210</v>
       </c>
       <c r="B39" s="24" t="s">
@@ -22566,7 +22376,7 @@
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="107"/>
+      <c r="A40" s="115"/>
       <c r="B40" s="64">
         <v>7200</v>
       </c>
@@ -22576,17 +22386,17 @@
       <c r="D40" s="64">
         <v>4800</v>
       </c>
-      <c r="F40" s="109" t="s">
+      <c r="F40" s="104" t="s">
         <v>218</v>
       </c>
-      <c r="G40" s="110"/>
-      <c r="I40" s="109" t="s">
+      <c r="G40" s="105"/>
+      <c r="I40" s="104" t="s">
         <v>252</v>
       </c>
-      <c r="J40" s="110"/>
+      <c r="J40" s="105"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="108"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="33">
         <f>ROUND(SQRT(B40),2)</f>
         <v>84.85</v>
@@ -22602,7 +22412,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A43" s="106" t="s">
+      <c r="A43" s="111" t="s">
         <v>137</v>
       </c>
       <c r="B43" s="44">
@@ -22649,7 +22459,7 @@
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A44" s="108"/>
+      <c r="A44" s="112"/>
       <c r="B44" s="29" t="s">
         <v>9</v>
       </c>
@@ -23201,7 +23011,7 @@
       <c r="K55" s="22"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="106" t="s">
+      <c r="A56" s="111" t="s">
         <v>141</v>
       </c>
       <c r="B56" s="44">
@@ -23242,7 +23052,7 @@
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="108"/>
+      <c r="A57" s="112"/>
       <c r="B57" s="29" t="s">
         <v>9</v>
       </c>
@@ -23774,7 +23584,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="106" t="s">
+      <c r="A69" s="111" t="s">
         <v>142</v>
       </c>
       <c r="B69" s="44">
@@ -23818,7 +23628,7 @@
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" s="108"/>
+      <c r="A70" s="112"/>
       <c r="B70" s="29" t="s">
         <v>9</v>
       </c>
@@ -24353,7 +24163,7 @@
       <c r="M80" s="58"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A82" s="106" t="s">
+      <c r="A82" s="111" t="s">
         <v>143</v>
       </c>
       <c r="B82" s="44">
@@ -24397,7 +24207,7 @@
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A83" s="108"/>
+      <c r="A83" s="112"/>
       <c r="B83" s="29" t="s">
         <v>9</v>
       </c>
@@ -24933,7 +24743,7 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A95" s="106" t="s">
+      <c r="A95" s="111" t="s">
         <v>144</v>
       </c>
       <c r="B95" s="44">
@@ -24977,7 +24787,7 @@
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A96" s="108"/>
+      <c r="A96" s="112"/>
       <c r="B96" s="29" t="s">
         <v>9</v>
       </c>
@@ -25513,7 +25323,7 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25"/>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A108" s="106" t="s">
+      <c r="A108" s="111" t="s">
         <v>145</v>
       </c>
       <c r="B108" s="44">
@@ -25557,7 +25367,7 @@
       </c>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A109" s="108"/>
+      <c r="A109" s="112"/>
       <c r="B109" s="29" t="s">
         <v>9</v>
       </c>
@@ -26093,7 +25903,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="121" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A121" s="106" t="s">
+      <c r="A121" s="111" t="s">
         <v>146</v>
       </c>
       <c r="B121" s="44">
@@ -26134,7 +25944,7 @@
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A122" s="108"/>
+      <c r="A122" s="112"/>
       <c r="B122" s="29" t="s">
         <v>9</v>
       </c>
@@ -26665,7 +26475,7 @@
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A134" s="106" t="s">
+      <c r="A134" s="111" t="s">
         <v>147</v>
       </c>
       <c r="B134" s="44">
@@ -26706,7 +26516,7 @@
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A135" s="108"/>
+      <c r="A135" s="112"/>
       <c r="B135" s="29" t="s">
         <v>9</v>
       </c>
@@ -27237,7 +27047,7 @@
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="147" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A147" s="106" t="s">
+      <c r="A147" s="111" t="s">
         <v>148</v>
       </c>
       <c r="B147" s="44">
@@ -27278,7 +27088,7 @@
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A148" s="108"/>
+      <c r="A148" s="112"/>
       <c r="B148" s="29" t="s">
         <v>9</v>
       </c>
@@ -27809,7 +27619,7 @@
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="160" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A160" s="106" t="s">
+      <c r="A160" s="111" t="s">
         <v>149</v>
       </c>
       <c r="B160" s="44">
@@ -27850,7 +27660,7 @@
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A161" s="108"/>
+      <c r="A161" s="112"/>
       <c r="B161" s="29" t="s">
         <v>9</v>
       </c>
@@ -28381,7 +28191,7 @@
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="173" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A173" s="106" t="s">
+      <c r="A173" s="111" t="s">
         <v>150</v>
       </c>
       <c r="B173" s="44">
@@ -28422,7 +28232,7 @@
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A174" s="108"/>
+      <c r="A174" s="112"/>
       <c r="B174" s="29" t="s">
         <v>9</v>
       </c>
@@ -28953,7 +28763,7 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.25"/>
     <row r="186" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A186" s="106" t="s">
+      <c r="A186" s="111" t="s">
         <v>151</v>
       </c>
       <c r="B186" s="44">
@@ -29000,7 +28810,7 @@
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A187" s="108"/>
+      <c r="A187" s="112"/>
       <c r="B187" s="29" t="s">
         <v>9</v>
       </c>
@@ -29539,7 +29349,7 @@
     </row>
     <row r="198" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="199" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A199" s="106" t="s">
+      <c r="A199" s="111" t="s">
         <v>152</v>
       </c>
       <c r="B199" s="44">
@@ -29580,7 +29390,7 @@
       </c>
     </row>
     <row r="200" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A200" s="108"/>
+      <c r="A200" s="112"/>
       <c r="B200" s="29" t="s">
         <v>9</v>
       </c>
@@ -30111,7 +29921,7 @@
     </row>
     <row r="211" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="212" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A212" s="106" t="s">
+      <c r="A212" s="111" t="s">
         <v>153</v>
       </c>
       <c r="B212" s="44">
@@ -30152,7 +29962,7 @@
       </c>
     </row>
     <row r="213" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A213" s="108"/>
+      <c r="A213" s="112"/>
       <c r="B213" s="29" t="s">
         <v>9</v>
       </c>
@@ -30682,7 +30492,7 @@
       </c>
     </row>
     <row r="225" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A225" s="106" t="s">
+      <c r="A225" s="111" t="s">
         <v>154</v>
       </c>
       <c r="B225" s="44">
@@ -30723,7 +30533,7 @@
       </c>
     </row>
     <row r="226" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A226" s="108"/>
+      <c r="A226" s="112"/>
       <c r="B226" s="29" t="s">
         <v>9</v>
       </c>
@@ -31254,7 +31064,7 @@
     </row>
     <row r="237" spans="1:14" x14ac:dyDescent="0.25"/>
     <row r="238" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A238" s="106" t="s">
+      <c r="A238" s="111" t="s">
         <v>155</v>
       </c>
       <c r="B238" s="44">
@@ -31295,7 +31105,7 @@
       </c>
     </row>
     <row r="239" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A239" s="108"/>
+      <c r="A239" s="112"/>
       <c r="B239" s="29" t="s">
         <v>9</v>
       </c>
@@ -31826,7 +31636,7 @@
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.25"/>
     <row r="251" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A251" s="106" t="s">
+      <c r="A251" s="111" t="s">
         <v>217</v>
       </c>
       <c r="B251" s="44">
@@ -31873,7 +31683,7 @@
       </c>
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A252" s="108"/>
+      <c r="A252" s="112"/>
       <c r="B252" s="29" t="s">
         <v>9</v>
       </c>
@@ -32433,7 +32243,7 @@
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="264" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A264" s="106" t="s">
+      <c r="A264" s="111" t="s">
         <v>222</v>
       </c>
       <c r="B264" s="69" t="s">
@@ -32486,7 +32296,7 @@
       </c>
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A265" s="108"/>
+      <c r="A265" s="112"/>
       <c r="B265" s="70" t="s">
         <v>221</v>
       </c>
@@ -32540,296 +32350,333 @@
       <c r="A266" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B266" s="111" t="s">
+      <c r="B266" s="110" t="s">
         <v>223</v>
       </c>
-      <c r="C266" s="111"/>
-      <c r="D266" s="111"/>
-      <c r="E266" s="111"/>
-      <c r="F266" s="111"/>
-      <c r="G266" s="111"/>
-      <c r="H266" s="111"/>
-      <c r="I266" s="111"/>
-      <c r="J266" s="111"/>
-      <c r="K266" s="111"/>
-      <c r="L266" s="111" t="s">
+      <c r="C266" s="110"/>
+      <c r="D266" s="110"/>
+      <c r="E266" s="110"/>
+      <c r="F266" s="110"/>
+      <c r="G266" s="110"/>
+      <c r="H266" s="110"/>
+      <c r="I266" s="110"/>
+      <c r="J266" s="110"/>
+      <c r="K266" s="110"/>
+      <c r="L266" s="110" t="s">
         <v>220</v>
       </c>
-      <c r="M266" s="111"/>
-      <c r="N266" s="111" t="s">
+      <c r="M266" s="110"/>
+      <c r="N266" s="110" t="s">
         <v>233</v>
       </c>
-      <c r="O266" s="111"/>
-      <c r="P266" s="111"/>
-      <c r="Q266" s="111"/>
+      <c r="O266" s="110"/>
+      <c r="P266" s="110"/>
+      <c r="Q266" s="110"/>
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A267" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B267" s="111" t="s">
+      <c r="B267" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="C267" s="111"/>
-      <c r="D267" s="111"/>
-      <c r="E267" s="111"/>
-      <c r="F267" s="111"/>
-      <c r="G267" s="111"/>
-      <c r="H267" s="111"/>
-      <c r="I267" s="111"/>
-      <c r="J267" s="111"/>
-      <c r="K267" s="111"/>
-      <c r="L267" s="111" t="s">
+      <c r="C267" s="110"/>
+      <c r="D267" s="110"/>
+      <c r="E267" s="110"/>
+      <c r="F267" s="110"/>
+      <c r="G267" s="110"/>
+      <c r="H267" s="110"/>
+      <c r="I267" s="110"/>
+      <c r="J267" s="110"/>
+      <c r="K267" s="110"/>
+      <c r="L267" s="110" t="s">
         <v>235</v>
       </c>
-      <c r="M267" s="111"/>
-      <c r="N267" s="111" t="s">
+      <c r="M267" s="110"/>
+      <c r="N267" s="110" t="s">
         <v>244</v>
       </c>
-      <c r="O267" s="111"/>
-      <c r="P267" s="111"/>
-      <c r="Q267" s="111"/>
+      <c r="O267" s="110"/>
+      <c r="P267" s="110"/>
+      <c r="Q267" s="110"/>
     </row>
     <row r="268" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A268" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B268" s="112" t="s">
+      <c r="B268" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="C268" s="113"/>
-      <c r="D268" s="113"/>
-      <c r="E268" s="113"/>
-      <c r="F268" s="113"/>
-      <c r="G268" s="113"/>
-      <c r="H268" s="113"/>
-      <c r="I268" s="113"/>
-      <c r="J268" s="113"/>
-      <c r="K268" s="114"/>
-      <c r="L268" s="111" t="s">
+      <c r="C268" s="108"/>
+      <c r="D268" s="108"/>
+      <c r="E268" s="108"/>
+      <c r="F268" s="108"/>
+      <c r="G268" s="108"/>
+      <c r="H268" s="108"/>
+      <c r="I268" s="108"/>
+      <c r="J268" s="108"/>
+      <c r="K268" s="109"/>
+      <c r="L268" s="110" t="s">
         <v>236</v>
       </c>
-      <c r="M268" s="111"/>
-      <c r="N268" s="111" t="s">
+      <c r="M268" s="110"/>
+      <c r="N268" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="O268" s="111"/>
-      <c r="P268" s="111"/>
-      <c r="Q268" s="111"/>
+      <c r="O268" s="110"/>
+      <c r="P268" s="110"/>
+      <c r="Q268" s="110"/>
     </row>
     <row r="269" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A269" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B269" s="112" t="s">
+      <c r="B269" s="107" t="s">
         <v>226</v>
       </c>
-      <c r="C269" s="113"/>
-      <c r="D269" s="113"/>
-      <c r="E269" s="113"/>
-      <c r="F269" s="113"/>
-      <c r="G269" s="113"/>
-      <c r="H269" s="113"/>
-      <c r="I269" s="113"/>
-      <c r="J269" s="113"/>
-      <c r="K269" s="114"/>
-      <c r="L269" s="111" t="s">
+      <c r="C269" s="108"/>
+      <c r="D269" s="108"/>
+      <c r="E269" s="108"/>
+      <c r="F269" s="108"/>
+      <c r="G269" s="108"/>
+      <c r="H269" s="108"/>
+      <c r="I269" s="108"/>
+      <c r="J269" s="108"/>
+      <c r="K269" s="109"/>
+      <c r="L269" s="110" t="s">
         <v>237</v>
       </c>
-      <c r="M269" s="111"/>
-      <c r="N269" s="111" t="s">
+      <c r="M269" s="110"/>
+      <c r="N269" s="110" t="s">
         <v>246</v>
       </c>
-      <c r="O269" s="111"/>
-      <c r="P269" s="111"/>
-      <c r="Q269" s="111"/>
+      <c r="O269" s="110"/>
+      <c r="P269" s="110"/>
+      <c r="Q269" s="110"/>
     </row>
     <row r="270" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A270" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B270" s="112" t="s">
+      <c r="B270" s="107" t="s">
         <v>227</v>
       </c>
-      <c r="C270" s="113"/>
-      <c r="D270" s="113"/>
-      <c r="E270" s="113"/>
-      <c r="F270" s="113"/>
-      <c r="G270" s="113"/>
-      <c r="H270" s="113"/>
-      <c r="I270" s="113"/>
-      <c r="J270" s="113"/>
-      <c r="K270" s="114"/>
-      <c r="L270" s="111" t="s">
+      <c r="C270" s="108"/>
+      <c r="D270" s="108"/>
+      <c r="E270" s="108"/>
+      <c r="F270" s="108"/>
+      <c r="G270" s="108"/>
+      <c r="H270" s="108"/>
+      <c r="I270" s="108"/>
+      <c r="J270" s="108"/>
+      <c r="K270" s="109"/>
+      <c r="L270" s="110" t="s">
         <v>238</v>
       </c>
-      <c r="M270" s="111"/>
-      <c r="N270" s="111" t="s">
+      <c r="M270" s="110"/>
+      <c r="N270" s="110" t="s">
         <v>247</v>
       </c>
-      <c r="O270" s="111"/>
-      <c r="P270" s="111"/>
-      <c r="Q270" s="111"/>
+      <c r="O270" s="110"/>
+      <c r="P270" s="110"/>
+      <c r="Q270" s="110"/>
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A271" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B271" s="112" t="s">
+      <c r="B271" s="107" t="s">
         <v>228</v>
       </c>
-      <c r="C271" s="113"/>
-      <c r="D271" s="113"/>
-      <c r="E271" s="113"/>
-      <c r="F271" s="113"/>
-      <c r="G271" s="113"/>
-      <c r="H271" s="113"/>
-      <c r="I271" s="113"/>
-      <c r="J271" s="113"/>
-      <c r="K271" s="114"/>
-      <c r="L271" s="111" t="s">
+      <c r="C271" s="108"/>
+      <c r="D271" s="108"/>
+      <c r="E271" s="108"/>
+      <c r="F271" s="108"/>
+      <c r="G271" s="108"/>
+      <c r="H271" s="108"/>
+      <c r="I271" s="108"/>
+      <c r="J271" s="108"/>
+      <c r="K271" s="109"/>
+      <c r="L271" s="110" t="s">
         <v>239</v>
       </c>
-      <c r="M271" s="111"/>
-      <c r="N271" s="111" t="s">
+      <c r="M271" s="110"/>
+      <c r="N271" s="110" t="s">
         <v>234</v>
       </c>
-      <c r="O271" s="111"/>
-      <c r="P271" s="111"/>
-      <c r="Q271" s="111"/>
+      <c r="O271" s="110"/>
+      <c r="P271" s="110"/>
+      <c r="Q271" s="110"/>
     </row>
     <row r="272" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A272" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B272" s="112" t="s">
+      <c r="B272" s="107" t="s">
         <v>229</v>
       </c>
-      <c r="C272" s="113"/>
-      <c r="D272" s="113"/>
-      <c r="E272" s="113"/>
-      <c r="F272" s="113"/>
-      <c r="G272" s="113"/>
-      <c r="H272" s="113"/>
-      <c r="I272" s="113"/>
-      <c r="J272" s="113"/>
-      <c r="K272" s="114"/>
-      <c r="L272" s="111" t="s">
+      <c r="C272" s="108"/>
+      <c r="D272" s="108"/>
+      <c r="E272" s="108"/>
+      <c r="F272" s="108"/>
+      <c r="G272" s="108"/>
+      <c r="H272" s="108"/>
+      <c r="I272" s="108"/>
+      <c r="J272" s="108"/>
+      <c r="K272" s="109"/>
+      <c r="L272" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="M272" s="111"/>
-      <c r="N272" s="111" t="s">
+      <c r="M272" s="110"/>
+      <c r="N272" s="110" t="s">
         <v>248</v>
       </c>
-      <c r="O272" s="111"/>
-      <c r="P272" s="111"/>
-      <c r="Q272" s="111"/>
+      <c r="O272" s="110"/>
+      <c r="P272" s="110"/>
+      <c r="Q272" s="110"/>
     </row>
     <row r="273" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A273" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B273" s="112" t="s">
+      <c r="B273" s="107" t="s">
         <v>230</v>
       </c>
-      <c r="C273" s="113"/>
-      <c r="D273" s="113"/>
-      <c r="E273" s="113"/>
-      <c r="F273" s="113"/>
-      <c r="G273" s="113"/>
-      <c r="H273" s="113"/>
-      <c r="I273" s="113"/>
-      <c r="J273" s="113"/>
-      <c r="K273" s="114"/>
-      <c r="L273" s="111" t="s">
+      <c r="C273" s="108"/>
+      <c r="D273" s="108"/>
+      <c r="E273" s="108"/>
+      <c r="F273" s="108"/>
+      <c r="G273" s="108"/>
+      <c r="H273" s="108"/>
+      <c r="I273" s="108"/>
+      <c r="J273" s="108"/>
+      <c r="K273" s="109"/>
+      <c r="L273" s="110" t="s">
         <v>241</v>
       </c>
-      <c r="M273" s="111"/>
-      <c r="N273" s="111" t="s">
+      <c r="M273" s="110"/>
+      <c r="N273" s="110" t="s">
         <v>249</v>
       </c>
-      <c r="O273" s="111"/>
-      <c r="P273" s="111"/>
-      <c r="Q273" s="111"/>
+      <c r="O273" s="110"/>
+      <c r="P273" s="110"/>
+      <c r="Q273" s="110"/>
     </row>
     <row r="274" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A274" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B274" s="112" t="s">
+      <c r="B274" s="107" t="s">
         <v>231</v>
       </c>
-      <c r="C274" s="113"/>
-      <c r="D274" s="113"/>
-      <c r="E274" s="113"/>
-      <c r="F274" s="113"/>
-      <c r="G274" s="113"/>
-      <c r="H274" s="113"/>
-      <c r="I274" s="113"/>
-      <c r="J274" s="113"/>
-      <c r="K274" s="114"/>
-      <c r="L274" s="111" t="s">
+      <c r="C274" s="108"/>
+      <c r="D274" s="108"/>
+      <c r="E274" s="108"/>
+      <c r="F274" s="108"/>
+      <c r="G274" s="108"/>
+      <c r="H274" s="108"/>
+      <c r="I274" s="108"/>
+      <c r="J274" s="108"/>
+      <c r="K274" s="109"/>
+      <c r="L274" s="110" t="s">
         <v>242</v>
       </c>
-      <c r="M274" s="111"/>
-      <c r="N274" s="111" t="s">
+      <c r="M274" s="110"/>
+      <c r="N274" s="110" t="s">
         <v>250</v>
       </c>
-      <c r="O274" s="111"/>
-      <c r="P274" s="111"/>
-      <c r="Q274" s="111"/>
+      <c r="O274" s="110"/>
+      <c r="P274" s="110"/>
+      <c r="Q274" s="110"/>
     </row>
     <row r="275" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A275" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B275" s="112" t="s">
+      <c r="B275" s="107" t="s">
         <v>232</v>
       </c>
-      <c r="C275" s="113"/>
-      <c r="D275" s="113"/>
-      <c r="E275" s="113"/>
-      <c r="F275" s="113"/>
-      <c r="G275" s="113"/>
-      <c r="H275" s="113"/>
-      <c r="I275" s="113"/>
-      <c r="J275" s="113"/>
-      <c r="K275" s="114"/>
-      <c r="L275" s="111" t="s">
+      <c r="C275" s="108"/>
+      <c r="D275" s="108"/>
+      <c r="E275" s="108"/>
+      <c r="F275" s="108"/>
+      <c r="G275" s="108"/>
+      <c r="H275" s="108"/>
+      <c r="I275" s="108"/>
+      <c r="J275" s="108"/>
+      <c r="K275" s="109"/>
+      <c r="L275" s="110" t="s">
         <v>243</v>
       </c>
-      <c r="M275" s="111"/>
-      <c r="N275" s="111" t="s">
+      <c r="M275" s="110"/>
+      <c r="N275" s="110" t="s">
         <v>251</v>
       </c>
-      <c r="O275" s="111"/>
-      <c r="P275" s="111"/>
-      <c r="Q275" s="111"/>
+      <c r="O275" s="110"/>
+      <c r="P275" s="110"/>
+      <c r="Q275" s="110"/>
     </row>
     <row r="276" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="277" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A277" s="115" t="s">
+      <c r="A277" s="106" t="s">
         <v>253</v>
       </c>
-      <c r="B277" s="115"/>
-      <c r="C277" s="115"/>
-      <c r="D277" s="115"/>
-      <c r="E277" s="115"/>
-      <c r="F277" s="115"/>
-      <c r="G277" s="115"/>
-      <c r="H277" s="115"/>
-      <c r="I277" s="115"/>
-      <c r="J277" s="115"/>
-      <c r="K277" s="115"/>
-      <c r="L277" s="115"/>
-      <c r="M277" s="115"/>
-      <c r="N277" s="115"/>
-      <c r="O277" s="115"/>
-      <c r="P277" s="115"/>
-      <c r="Q277" s="115"/>
+      <c r="B277" s="106"/>
+      <c r="C277" s="106"/>
+      <c r="D277" s="106"/>
+      <c r="E277" s="106"/>
+      <c r="F277" s="106"/>
+      <c r="G277" s="106"/>
+      <c r="H277" s="106"/>
+      <c r="I277" s="106"/>
+      <c r="J277" s="106"/>
+      <c r="K277" s="106"/>
+      <c r="L277" s="106"/>
+      <c r="M277" s="106"/>
+      <c r="N277" s="106"/>
+      <c r="O277" s="106"/>
+      <c r="P277" s="106"/>
+      <c r="Q277" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A134:A135"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A108:A109"/>
+    <mergeCell ref="A251:A252"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="A199:A200"/>
+    <mergeCell ref="A212:A213"/>
+    <mergeCell ref="A225:A226"/>
+    <mergeCell ref="A238:A239"/>
+    <mergeCell ref="A160:A161"/>
+    <mergeCell ref="A173:A174"/>
+    <mergeCell ref="A186:A187"/>
+    <mergeCell ref="A264:A265"/>
+    <mergeCell ref="B266:K266"/>
+    <mergeCell ref="L266:M266"/>
+    <mergeCell ref="N266:Q266"/>
+    <mergeCell ref="B267:K267"/>
+    <mergeCell ref="L267:M267"/>
+    <mergeCell ref="N267:Q267"/>
+    <mergeCell ref="N270:Q270"/>
+    <mergeCell ref="B271:K271"/>
+    <mergeCell ref="L271:M271"/>
+    <mergeCell ref="N271:Q271"/>
+    <mergeCell ref="B268:K268"/>
+    <mergeCell ref="L268:M268"/>
+    <mergeCell ref="N268:Q268"/>
+    <mergeCell ref="B269:K269"/>
+    <mergeCell ref="L269:M269"/>
+    <mergeCell ref="N269:Q269"/>
     <mergeCell ref="I40:J40"/>
     <mergeCell ref="A277:Q277"/>
     <mergeCell ref="B274:K274"/>
@@ -32846,43 +32693,6 @@
     <mergeCell ref="N273:Q273"/>
     <mergeCell ref="B270:K270"/>
     <mergeCell ref="L270:M270"/>
-    <mergeCell ref="N270:Q270"/>
-    <mergeCell ref="B271:K271"/>
-    <mergeCell ref="L271:M271"/>
-    <mergeCell ref="N271:Q271"/>
-    <mergeCell ref="B268:K268"/>
-    <mergeCell ref="L268:M268"/>
-    <mergeCell ref="N268:Q268"/>
-    <mergeCell ref="B269:K269"/>
-    <mergeCell ref="L269:M269"/>
-    <mergeCell ref="N269:Q269"/>
-    <mergeCell ref="A264:A265"/>
-    <mergeCell ref="B266:K266"/>
-    <mergeCell ref="L266:M266"/>
-    <mergeCell ref="N266:Q266"/>
-    <mergeCell ref="B267:K267"/>
-    <mergeCell ref="L267:M267"/>
-    <mergeCell ref="N267:Q267"/>
-    <mergeCell ref="A251:A252"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="A199:A200"/>
-    <mergeCell ref="A212:A213"/>
-    <mergeCell ref="A225:A226"/>
-    <mergeCell ref="A238:A239"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="A173:A174"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A108:A109"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N43" location="'Ranged Weapon'!B1" display="Damage Stat" xr:uid="{41986C71-802E-4E5D-9AB0-D4A5C3E2EAE6}"/>
@@ -32940,7 +32750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7B0F5C-DCD6-460C-8032-B8DBD5D38B94}">
   <dimension ref="A1:V282"/>
   <sheetViews>
@@ -32957,7 +32767,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="113" t="s">
         <v>156</v>
       </c>
       <c r="B1" s="62" t="s">
@@ -33010,7 +32820,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="105"/>
+      <c r="A2" s="114"/>
       <c r="B2" s="63">
         <v>100</v>
       </c>
@@ -35168,7 +34978,7 @@
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25"/>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="106" t="s">
+      <c r="A42" s="111" t="s">
         <v>210</v>
       </c>
       <c r="B42" s="24" t="s">
@@ -35182,7 +34992,7 @@
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="107"/>
+      <c r="A43" s="115"/>
       <c r="B43" s="64">
         <v>50000</v>
       </c>
@@ -35192,17 +35002,17 @@
       <c r="D43" s="64">
         <v>50000</v>
       </c>
-      <c r="F43" s="109" t="s">
+      <c r="F43" s="104" t="s">
         <v>218</v>
       </c>
-      <c r="G43" s="110"/>
-      <c r="I43" s="109" t="s">
+      <c r="G43" s="105"/>
+      <c r="I43" s="104" t="s">
         <v>252</v>
       </c>
-      <c r="J43" s="110"/>
+      <c r="J43" s="105"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="108"/>
+      <c r="A44" s="112"/>
       <c r="B44" s="33">
         <f>ROUND(SQRT(B43),2)</f>
         <v>223.61</v>
@@ -35218,7 +35028,7 @@
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46" s="106" t="s">
+      <c r="A46" s="111" t="s">
         <v>137</v>
       </c>
       <c r="B46" s="44">
@@ -35274,7 +35084,7 @@
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47" s="108"/>
+      <c r="A47" s="112"/>
       <c r="B47" s="29" t="s">
         <v>29</v>
       </c>
@@ -35942,7 +35752,7 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" s="106" t="s">
+      <c r="A59" s="111" t="s">
         <v>168</v>
       </c>
       <c r="B59" s="44">
@@ -35992,7 +35802,7 @@
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A60" s="108"/>
+      <c r="A60" s="112"/>
       <c r="B60" s="29" t="s">
         <v>29</v>
       </c>
@@ -36652,7 +36462,7 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25"/>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A72" s="106" t="s">
+      <c r="A72" s="111" t="s">
         <v>142</v>
       </c>
       <c r="B72" s="44">
@@ -36705,7 +36515,7 @@
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A73" s="108"/>
+      <c r="A73" s="112"/>
       <c r="B73" s="29" t="s">
         <v>29</v>
       </c>
@@ -37369,7 +37179,7 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25"/>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A85" s="106" t="s">
+      <c r="A85" s="111" t="s">
         <v>143</v>
       </c>
       <c r="B85" s="44">
@@ -37422,7 +37232,7 @@
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A86" s="108"/>
+      <c r="A86" s="112"/>
       <c r="B86" s="29" t="s">
         <v>29</v>
       </c>
@@ -38086,7 +37896,7 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25"/>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A99" s="106" t="s">
+      <c r="A99" s="111" t="s">
         <v>172</v>
       </c>
       <c r="B99" s="44">
@@ -38136,7 +37946,7 @@
       </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A100" s="108"/>
+      <c r="A100" s="112"/>
       <c r="B100" s="29" t="s">
         <v>29</v>
       </c>
@@ -38796,7 +38606,7 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25"/>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A112" s="106" t="s">
+      <c r="A112" s="111" t="s">
         <v>173</v>
       </c>
       <c r="B112" s="44">
@@ -38849,7 +38659,7 @@
       </c>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A113" s="108"/>
+      <c r="A113" s="112"/>
       <c r="B113" s="29" t="s">
         <v>29</v>
       </c>
@@ -39513,7 +39323,7 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25"/>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A125" s="106" t="s">
+      <c r="A125" s="111" t="s">
         <v>181</v>
       </c>
       <c r="B125" s="44">
@@ -39563,7 +39373,7 @@
       </c>
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A126" s="108"/>
+      <c r="A126" s="112"/>
       <c r="B126" s="29" t="s">
         <v>29</v>
       </c>
@@ -40223,7 +40033,7 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="138" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A138" s="106" t="s">
+      <c r="A138" s="111" t="s">
         <v>174</v>
       </c>
       <c r="B138" s="44">
@@ -40273,7 +40083,7 @@
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A139" s="108"/>
+      <c r="A139" s="112"/>
       <c r="B139" s="29" t="s">
         <v>29</v>
       </c>
@@ -40933,7 +40743,7 @@
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A151" s="106" t="s">
+      <c r="A151" s="111" t="s">
         <v>148</v>
       </c>
       <c r="B151" s="44">
@@ -40983,7 +40793,7 @@
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A152" s="108"/>
+      <c r="A152" s="112"/>
       <c r="B152" s="29" t="s">
         <v>29</v>
       </c>
@@ -41643,7 +41453,7 @@
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="164" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A164" s="106" t="s">
+      <c r="A164" s="111" t="s">
         <v>149</v>
       </c>
       <c r="B164" s="44">
@@ -41693,7 +41503,7 @@
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A165" s="108"/>
+      <c r="A165" s="112"/>
       <c r="B165" s="29" t="s">
         <v>29</v>
       </c>
@@ -42353,7 +42163,7 @@
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="177" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A177" s="106" t="s">
+      <c r="A177" s="111" t="s">
         <v>150</v>
       </c>
       <c r="B177" s="44">
@@ -42403,7 +42213,7 @@
       </c>
     </row>
     <row r="178" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A178" s="108"/>
+      <c r="A178" s="112"/>
       <c r="B178" s="29" t="s">
         <v>29</v>
       </c>
@@ -43063,7 +42873,7 @@
     </row>
     <row r="189" spans="1:19" x14ac:dyDescent="0.25"/>
     <row r="190" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A190" s="106" t="s">
+      <c r="A190" s="111" t="s">
         <v>211</v>
       </c>
       <c r="B190" s="44">
@@ -43119,7 +42929,7 @@
       </c>
     </row>
     <row r="191" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A191" s="108"/>
+      <c r="A191" s="112"/>
       <c r="B191" s="29" t="s">
         <v>29</v>
       </c>
@@ -43787,7 +43597,7 @@
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="203" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A203" s="106" t="s">
+      <c r="A203" s="111" t="s">
         <v>212</v>
       </c>
       <c r="B203" s="44">
@@ -43837,7 +43647,7 @@
       </c>
     </row>
     <row r="204" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A204" s="108"/>
+      <c r="A204" s="112"/>
       <c r="B204" s="29" t="s">
         <v>29</v>
       </c>
@@ -44497,7 +44307,7 @@
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="216" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A216" s="106" t="s">
+      <c r="A216" s="111" t="s">
         <v>213</v>
       </c>
       <c r="B216" s="44">
@@ -44547,7 +44357,7 @@
       </c>
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A217" s="108"/>
+      <c r="A217" s="112"/>
       <c r="B217" s="29" t="s">
         <v>29</v>
       </c>
@@ -45207,7 +45017,7 @@
     </row>
     <row r="228" spans="1:17" x14ac:dyDescent="0.25"/>
     <row r="229" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A229" s="106" t="s">
+      <c r="A229" s="111" t="s">
         <v>214</v>
       </c>
       <c r="B229" s="44">
@@ -45257,7 +45067,7 @@
       </c>
     </row>
     <row r="230" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A230" s="108"/>
+      <c r="A230" s="112"/>
       <c r="B230" s="29" t="s">
         <v>29</v>
       </c>
@@ -45917,7 +45727,7 @@
     </row>
     <row r="242" spans="1:19" x14ac:dyDescent="0.25"/>
     <row r="243" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A243" s="106" t="s">
+      <c r="A243" s="111" t="s">
         <v>215</v>
       </c>
       <c r="B243" s="44">
@@ -45967,7 +45777,7 @@
       </c>
     </row>
     <row r="244" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A244" s="108"/>
+      <c r="A244" s="112"/>
       <c r="B244" s="29" t="s">
         <v>29</v>
       </c>
@@ -46627,7 +46437,7 @@
     </row>
     <row r="255" spans="1:19" x14ac:dyDescent="0.25"/>
     <row r="256" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A256" s="106" t="s">
+      <c r="A256" s="111" t="s">
         <v>219</v>
       </c>
       <c r="B256" s="44">
@@ -46683,7 +46493,7 @@
       </c>
     </row>
     <row r="257" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A257" s="108"/>
+      <c r="A257" s="112"/>
       <c r="B257" s="29" t="s">
         <v>29</v>
       </c>
@@ -47372,7 +47182,7 @@
     </row>
     <row r="268" spans="1:19" x14ac:dyDescent="0.25"/>
     <row r="269" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A269" s="106" t="s">
+      <c r="A269" s="111" t="s">
         <v>222</v>
       </c>
       <c r="B269" s="69" t="s">
@@ -47425,7 +47235,7 @@
       </c>
     </row>
     <row r="270" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A270" s="108"/>
+      <c r="A270" s="112"/>
       <c r="B270" s="70" t="s">
         <v>221</v>
       </c>
@@ -47479,298 +47289,335 @@
       <c r="A271" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="B271" s="111" t="s">
+      <c r="B271" s="110" t="s">
         <v>223</v>
       </c>
-      <c r="C271" s="111"/>
-      <c r="D271" s="111"/>
-      <c r="E271" s="111"/>
-      <c r="F271" s="111"/>
-      <c r="G271" s="111"/>
-      <c r="H271" s="111"/>
-      <c r="I271" s="111"/>
-      <c r="J271" s="111"/>
-      <c r="K271" s="111"/>
-      <c r="L271" s="111" t="s">
+      <c r="C271" s="110"/>
+      <c r="D271" s="110"/>
+      <c r="E271" s="110"/>
+      <c r="F271" s="110"/>
+      <c r="G271" s="110"/>
+      <c r="H271" s="110"/>
+      <c r="I271" s="110"/>
+      <c r="J271" s="110"/>
+      <c r="K271" s="110"/>
+      <c r="L271" s="110" t="s">
         <v>220</v>
       </c>
-      <c r="M271" s="111"/>
-      <c r="N271" s="111" t="s">
+      <c r="M271" s="110"/>
+      <c r="N271" s="110" t="s">
         <v>233</v>
       </c>
-      <c r="O271" s="111"/>
-      <c r="P271" s="111"/>
-      <c r="Q271" s="111"/>
+      <c r="O271" s="110"/>
+      <c r="P271" s="110"/>
+      <c r="Q271" s="110"/>
     </row>
     <row r="272" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A272" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="B272" s="111" t="s">
+      <c r="B272" s="110" t="s">
         <v>224</v>
       </c>
-      <c r="C272" s="111"/>
-      <c r="D272" s="111"/>
-      <c r="E272" s="111"/>
-      <c r="F272" s="111"/>
-      <c r="G272" s="111"/>
-      <c r="H272" s="111"/>
-      <c r="I272" s="111"/>
-      <c r="J272" s="111"/>
-      <c r="K272" s="111"/>
-      <c r="L272" s="111" t="s">
+      <c r="C272" s="110"/>
+      <c r="D272" s="110"/>
+      <c r="E272" s="110"/>
+      <c r="F272" s="110"/>
+      <c r="G272" s="110"/>
+      <c r="H272" s="110"/>
+      <c r="I272" s="110"/>
+      <c r="J272" s="110"/>
+      <c r="K272" s="110"/>
+      <c r="L272" s="110" t="s">
         <v>235</v>
       </c>
-      <c r="M272" s="111"/>
-      <c r="N272" s="111" t="s">
+      <c r="M272" s="110"/>
+      <c r="N272" s="110" t="s">
         <v>244</v>
       </c>
-      <c r="O272" s="111"/>
-      <c r="P272" s="111"/>
-      <c r="Q272" s="111"/>
+      <c r="O272" s="110"/>
+      <c r="P272" s="110"/>
+      <c r="Q272" s="110"/>
     </row>
     <row r="273" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A273" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B273" s="112" t="s">
+      <c r="B273" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="C273" s="113"/>
-      <c r="D273" s="113"/>
-      <c r="E273" s="113"/>
-      <c r="F273" s="113"/>
-      <c r="G273" s="113"/>
-      <c r="H273" s="113"/>
-      <c r="I273" s="113"/>
-      <c r="J273" s="113"/>
-      <c r="K273" s="114"/>
-      <c r="L273" s="111" t="s">
+      <c r="C273" s="108"/>
+      <c r="D273" s="108"/>
+      <c r="E273" s="108"/>
+      <c r="F273" s="108"/>
+      <c r="G273" s="108"/>
+      <c r="H273" s="108"/>
+      <c r="I273" s="108"/>
+      <c r="J273" s="108"/>
+      <c r="K273" s="109"/>
+      <c r="L273" s="110" t="s">
         <v>236</v>
       </c>
-      <c r="M273" s="111"/>
-      <c r="N273" s="111" t="s">
+      <c r="M273" s="110"/>
+      <c r="N273" s="110" t="s">
         <v>245</v>
       </c>
-      <c r="O273" s="111"/>
-      <c r="P273" s="111"/>
-      <c r="Q273" s="111"/>
+      <c r="O273" s="110"/>
+      <c r="P273" s="110"/>
+      <c r="Q273" s="110"/>
     </row>
     <row r="274" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A274" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B274" s="112" t="s">
+      <c r="B274" s="107" t="s">
         <v>226</v>
       </c>
-      <c r="C274" s="113"/>
-      <c r="D274" s="113"/>
-      <c r="E274" s="113"/>
-      <c r="F274" s="113"/>
-      <c r="G274" s="113"/>
-      <c r="H274" s="113"/>
-      <c r="I274" s="113"/>
-      <c r="J274" s="113"/>
-      <c r="K274" s="114"/>
-      <c r="L274" s="111" t="s">
+      <c r="C274" s="108"/>
+      <c r="D274" s="108"/>
+      <c r="E274" s="108"/>
+      <c r="F274" s="108"/>
+      <c r="G274" s="108"/>
+      <c r="H274" s="108"/>
+      <c r="I274" s="108"/>
+      <c r="J274" s="108"/>
+      <c r="K274" s="109"/>
+      <c r="L274" s="110" t="s">
         <v>237</v>
       </c>
-      <c r="M274" s="111"/>
-      <c r="N274" s="111" t="s">
+      <c r="M274" s="110"/>
+      <c r="N274" s="110" t="s">
         <v>246</v>
       </c>
-      <c r="O274" s="111"/>
-      <c r="P274" s="111"/>
-      <c r="Q274" s="111"/>
+      <c r="O274" s="110"/>
+      <c r="P274" s="110"/>
+      <c r="Q274" s="110"/>
     </row>
     <row r="275" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A275" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B275" s="112" t="s">
+      <c r="B275" s="107" t="s">
         <v>227</v>
       </c>
-      <c r="C275" s="113"/>
-      <c r="D275" s="113"/>
-      <c r="E275" s="113"/>
-      <c r="F275" s="113"/>
-      <c r="G275" s="113"/>
-      <c r="H275" s="113"/>
-      <c r="I275" s="113"/>
-      <c r="J275" s="113"/>
-      <c r="K275" s="114"/>
-      <c r="L275" s="111" t="s">
+      <c r="C275" s="108"/>
+      <c r="D275" s="108"/>
+      <c r="E275" s="108"/>
+      <c r="F275" s="108"/>
+      <c r="G275" s="108"/>
+      <c r="H275" s="108"/>
+      <c r="I275" s="108"/>
+      <c r="J275" s="108"/>
+      <c r="K275" s="109"/>
+      <c r="L275" s="110" t="s">
         <v>238</v>
       </c>
-      <c r="M275" s="111"/>
-      <c r="N275" s="111" t="s">
+      <c r="M275" s="110"/>
+      <c r="N275" s="110" t="s">
         <v>247</v>
       </c>
-      <c r="O275" s="111"/>
-      <c r="P275" s="111"/>
-      <c r="Q275" s="111"/>
+      <c r="O275" s="110"/>
+      <c r="P275" s="110"/>
+      <c r="Q275" s="110"/>
     </row>
     <row r="276" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A276" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="B276" s="112" t="s">
+      <c r="B276" s="107" t="s">
         <v>228</v>
       </c>
-      <c r="C276" s="113"/>
-      <c r="D276" s="113"/>
-      <c r="E276" s="113"/>
-      <c r="F276" s="113"/>
-      <c r="G276" s="113"/>
-      <c r="H276" s="113"/>
-      <c r="I276" s="113"/>
-      <c r="J276" s="113"/>
-      <c r="K276" s="114"/>
-      <c r="L276" s="111" t="s">
+      <c r="C276" s="108"/>
+      <c r="D276" s="108"/>
+      <c r="E276" s="108"/>
+      <c r="F276" s="108"/>
+      <c r="G276" s="108"/>
+      <c r="H276" s="108"/>
+      <c r="I276" s="108"/>
+      <c r="J276" s="108"/>
+      <c r="K276" s="109"/>
+      <c r="L276" s="110" t="s">
         <v>239</v>
       </c>
-      <c r="M276" s="111"/>
-      <c r="N276" s="111" t="s">
+      <c r="M276" s="110"/>
+      <c r="N276" s="110" t="s">
         <v>234</v>
       </c>
-      <c r="O276" s="111"/>
-      <c r="P276" s="111"/>
-      <c r="Q276" s="111"/>
+      <c r="O276" s="110"/>
+      <c r="P276" s="110"/>
+      <c r="Q276" s="110"/>
     </row>
     <row r="277" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A277" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B277" s="112" t="s">
+      <c r="B277" s="107" t="s">
         <v>229</v>
       </c>
-      <c r="C277" s="113"/>
-      <c r="D277" s="113"/>
-      <c r="E277" s="113"/>
-      <c r="F277" s="113"/>
-      <c r="G277" s="113"/>
-      <c r="H277" s="113"/>
-      <c r="I277" s="113"/>
-      <c r="J277" s="113"/>
-      <c r="K277" s="114"/>
-      <c r="L277" s="111" t="s">
+      <c r="C277" s="108"/>
+      <c r="D277" s="108"/>
+      <c r="E277" s="108"/>
+      <c r="F277" s="108"/>
+      <c r="G277" s="108"/>
+      <c r="H277" s="108"/>
+      <c r="I277" s="108"/>
+      <c r="J277" s="108"/>
+      <c r="K277" s="109"/>
+      <c r="L277" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="M277" s="111"/>
-      <c r="N277" s="111" t="s">
+      <c r="M277" s="110"/>
+      <c r="N277" s="110" t="s">
         <v>248</v>
       </c>
-      <c r="O277" s="111"/>
-      <c r="P277" s="111"/>
-      <c r="Q277" s="111"/>
+      <c r="O277" s="110"/>
+      <c r="P277" s="110"/>
+      <c r="Q277" s="110"/>
     </row>
     <row r="278" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A278" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B278" s="112" t="s">
+      <c r="B278" s="107" t="s">
         <v>230</v>
       </c>
-      <c r="C278" s="113"/>
-      <c r="D278" s="113"/>
-      <c r="E278" s="113"/>
-      <c r="F278" s="113"/>
-      <c r="G278" s="113"/>
-      <c r="H278" s="113"/>
-      <c r="I278" s="113"/>
-      <c r="J278" s="113"/>
-      <c r="K278" s="114"/>
-      <c r="L278" s="111" t="s">
+      <c r="C278" s="108"/>
+      <c r="D278" s="108"/>
+      <c r="E278" s="108"/>
+      <c r="F278" s="108"/>
+      <c r="G278" s="108"/>
+      <c r="H278" s="108"/>
+      <c r="I278" s="108"/>
+      <c r="J278" s="108"/>
+      <c r="K278" s="109"/>
+      <c r="L278" s="110" t="s">
         <v>241</v>
       </c>
-      <c r="M278" s="111"/>
-      <c r="N278" s="111" t="s">
+      <c r="M278" s="110"/>
+      <c r="N278" s="110" t="s">
         <v>249</v>
       </c>
-      <c r="O278" s="111"/>
-      <c r="P278" s="111"/>
-      <c r="Q278" s="111"/>
+      <c r="O278" s="110"/>
+      <c r="P278" s="110"/>
+      <c r="Q278" s="110"/>
     </row>
     <row r="279" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A279" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B279" s="112" t="s">
+      <c r="B279" s="107" t="s">
         <v>231</v>
       </c>
-      <c r="C279" s="113"/>
-      <c r="D279" s="113"/>
-      <c r="E279" s="113"/>
-      <c r="F279" s="113"/>
-      <c r="G279" s="113"/>
-      <c r="H279" s="113"/>
-      <c r="I279" s="113"/>
-      <c r="J279" s="113"/>
-      <c r="K279" s="114"/>
-      <c r="L279" s="111" t="s">
+      <c r="C279" s="108"/>
+      <c r="D279" s="108"/>
+      <c r="E279" s="108"/>
+      <c r="F279" s="108"/>
+      <c r="G279" s="108"/>
+      <c r="H279" s="108"/>
+      <c r="I279" s="108"/>
+      <c r="J279" s="108"/>
+      <c r="K279" s="109"/>
+      <c r="L279" s="110" t="s">
         <v>242</v>
       </c>
-      <c r="M279" s="111"/>
-      <c r="N279" s="111" t="s">
+      <c r="M279" s="110"/>
+      <c r="N279" s="110" t="s">
         <v>250</v>
       </c>
-      <c r="O279" s="111"/>
-      <c r="P279" s="111"/>
-      <c r="Q279" s="111"/>
+      <c r="O279" s="110"/>
+      <c r="P279" s="110"/>
+      <c r="Q279" s="110"/>
     </row>
     <row r="280" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A280" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B280" s="112" t="s">
+      <c r="B280" s="107" t="s">
         <v>232</v>
       </c>
-      <c r="C280" s="113"/>
-      <c r="D280" s="113"/>
-      <c r="E280" s="113"/>
-      <c r="F280" s="113"/>
-      <c r="G280" s="113"/>
-      <c r="H280" s="113"/>
-      <c r="I280" s="113"/>
-      <c r="J280" s="113"/>
-      <c r="K280" s="114"/>
-      <c r="L280" s="111" t="s">
+      <c r="C280" s="108"/>
+      <c r="D280" s="108"/>
+      <c r="E280" s="108"/>
+      <c r="F280" s="108"/>
+      <c r="G280" s="108"/>
+      <c r="H280" s="108"/>
+      <c r="I280" s="108"/>
+      <c r="J280" s="108"/>
+      <c r="K280" s="109"/>
+      <c r="L280" s="110" t="s">
         <v>243</v>
       </c>
-      <c r="M280" s="111"/>
-      <c r="N280" s="111" t="s">
+      <c r="M280" s="110"/>
+      <c r="N280" s="110" t="s">
         <v>251</v>
       </c>
-      <c r="O280" s="111"/>
-      <c r="P280" s="111"/>
-      <c r="Q280" s="111"/>
+      <c r="O280" s="110"/>
+      <c r="P280" s="110"/>
+      <c r="Q280" s="110"/>
     </row>
     <row r="281" spans="1:19" x14ac:dyDescent="0.25"/>
     <row r="282" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A282" s="115" t="s">
+      <c r="A282" s="106" t="s">
         <v>253</v>
       </c>
-      <c r="B282" s="115"/>
-      <c r="C282" s="115"/>
-      <c r="D282" s="115"/>
-      <c r="E282" s="115"/>
-      <c r="F282" s="115"/>
-      <c r="G282" s="115"/>
-      <c r="H282" s="115"/>
-      <c r="I282" s="115"/>
-      <c r="J282" s="115"/>
-      <c r="K282" s="115"/>
-      <c r="L282" s="115"/>
-      <c r="M282" s="115"/>
-      <c r="N282" s="115"/>
-      <c r="O282" s="115"/>
-      <c r="P282" s="115"/>
-      <c r="Q282" s="115"/>
-      <c r="R282" s="115"/>
-      <c r="S282" s="115"/>
+      <c r="B282" s="106"/>
+      <c r="C282" s="106"/>
+      <c r="D282" s="106"/>
+      <c r="E282" s="106"/>
+      <c r="F282" s="106"/>
+      <c r="G282" s="106"/>
+      <c r="H282" s="106"/>
+      <c r="I282" s="106"/>
+      <c r="J282" s="106"/>
+      <c r="K282" s="106"/>
+      <c r="L282" s="106"/>
+      <c r="M282" s="106"/>
+      <c r="N282" s="106"/>
+      <c r="O282" s="106"/>
+      <c r="P282" s="106"/>
+      <c r="Q282" s="106"/>
+      <c r="R282" s="106"/>
+      <c r="S282" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A216:A217"/>
+    <mergeCell ref="A229:A230"/>
+    <mergeCell ref="A243:A244"/>
+    <mergeCell ref="A256:A257"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="A164:A165"/>
+    <mergeCell ref="A177:A178"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="A203:A204"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="A138:A139"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="A269:A270"/>
+    <mergeCell ref="B271:K271"/>
+    <mergeCell ref="L271:M271"/>
+    <mergeCell ref="N271:Q271"/>
+    <mergeCell ref="B272:K272"/>
+    <mergeCell ref="L272:M272"/>
+    <mergeCell ref="N272:Q272"/>
+    <mergeCell ref="N275:Q275"/>
+    <mergeCell ref="B276:K276"/>
+    <mergeCell ref="L276:M276"/>
+    <mergeCell ref="N276:Q276"/>
+    <mergeCell ref="B273:K273"/>
+    <mergeCell ref="L273:M273"/>
+    <mergeCell ref="N273:Q273"/>
+    <mergeCell ref="B274:K274"/>
+    <mergeCell ref="L274:M274"/>
+    <mergeCell ref="N274:Q274"/>
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="A282:S282"/>
     <mergeCell ref="B279:K279"/>
@@ -47787,43 +47634,6 @@
     <mergeCell ref="N278:Q278"/>
     <mergeCell ref="B275:K275"/>
     <mergeCell ref="L275:M275"/>
-    <mergeCell ref="N275:Q275"/>
-    <mergeCell ref="B276:K276"/>
-    <mergeCell ref="L276:M276"/>
-    <mergeCell ref="N276:Q276"/>
-    <mergeCell ref="B273:K273"/>
-    <mergeCell ref="L273:M273"/>
-    <mergeCell ref="N273:Q273"/>
-    <mergeCell ref="B274:K274"/>
-    <mergeCell ref="L274:M274"/>
-    <mergeCell ref="N274:Q274"/>
-    <mergeCell ref="A269:A270"/>
-    <mergeCell ref="B271:K271"/>
-    <mergeCell ref="L271:M271"/>
-    <mergeCell ref="N271:Q271"/>
-    <mergeCell ref="B272:K272"/>
-    <mergeCell ref="L272:M272"/>
-    <mergeCell ref="N272:Q272"/>
-    <mergeCell ref="A243:A244"/>
-    <mergeCell ref="A256:A257"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="A151:A152"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="A177:A178"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="A203:A204"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="A216:A217"/>
-    <mergeCell ref="A229:A230"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>